<commit_message>
resnet 200 data/graphs 10 gbps, in rack, uneven, striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/resnet-200/graphs/10gbps_inrack_uneven_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/resnet-200/graphs/10gbps_inrack_uneven_striping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -261,19 +258,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>11.2164</c:v>
+                    <c:v>8.1264</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3721</c:v>
+                    <c:v>0.3162</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.2229</c:v>
+                    <c:v>2.0525</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2517</c:v>
+                    <c:v>0.1233</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8762</c:v>
+                    <c:v>0.8055</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -285,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0109</c:v>
+                    <c:v>0.008</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2003</c:v>
+                    <c:v>0.1703</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.3802</c:v>
+                    <c:v>8.7206</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9919</c:v>
+                    <c:v>1.8375</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.99</c:v>
+                    <c:v>0.4504</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -350,16 +347,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.2891</c:v>
+                  <c:v>18.0912</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.902</c:v>
+                  <c:v>31.5302</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.7117</c:v>
+                  <c:v>39.9193</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.345</c:v>
+                  <c:v>43.356</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,19 +405,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1164</c:v>
+                    <c:v>0.3727</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.084</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.6705</c:v>
+                    <c:v>5.9689</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.324</c:v>
+                    <c:v>1.1154</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.1987</c:v>
+                    <c:v>0.235</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -432,19 +429,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2233</c:v>
+                    <c:v>0.2633</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0419</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>20.1291</c:v>
+                    <c:v>19.7955</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.8769</c:v>
+                    <c:v>2.5691</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.3436</c:v>
+                    <c:v>1.934</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -494,19 +491,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-0.1261</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.3472</c:v>
+                  <c:v>22.0488</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.8608</c:v>
+                  <c:v>35.2189</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.6138</c:v>
+                  <c:v>42.707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,16 +555,16 @@
                     <c:v>0.1534</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.242</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.1767</c:v>
+                    <c:v>4.4358</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4928</c:v>
+                    <c:v>0.8663</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.415</c:v>
+                    <c:v>1.4904</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -579,19 +576,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.169</c:v>
+                    <c:v>0.1839</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.1827</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>12.0289</c:v>
+                    <c:v>10.7309</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.9001</c:v>
+                    <c:v>5.5403</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2189</c:v>
+                    <c:v>1.8046</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -641,19 +638,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.1013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.9592</c:v>
+                  <c:v>10.6767</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.2959</c:v>
+                  <c:v>29.6527</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.7364</c:v>
+                  <c:v>38.5069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,19 +699,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6518</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.52</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.0775</c:v>
+                    <c:v>5.0168</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.8192</c:v>
+                    <c:v>0.2315</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4113</c:v>
+                    <c:v>2.1031</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -726,19 +723,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6891</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.4075</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>11.7638</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.782199999999999</c:v>
+                    <c:v>4.3144</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.3163</c:v>
+                    <c:v>1.5921</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -788,19 +785,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.4075</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11.6939</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.4788</c:v>
+                  <c:v>30.4207</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.6332</c:v>
+                  <c:v>38.0358</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080204368"/>
-        <c:axId val="-2080198144"/>
+        <c:axId val="-2096944608"/>
+        <c:axId val="-2096952672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2080204368"/>
+        <c:axId val="-2096944608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080198144"/>
+        <c:crossAx val="-2096952672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2080198144"/>
+        <c:axId val="-2096952672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080204368"/>
+        <c:crossAx val="-2096944608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,19 +1290,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0914</c:v>
+                    <c:v>0.5715</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2956</c:v>
+                    <c:v>0.3142</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.5567</c:v>
+                    <c:v>0.9646</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1405</c:v>
+                    <c:v>0.2582</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1317,19 +1314,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.6253</c:v>
+                    <c:v>0.083</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.264</c:v>
+                    <c:v>0.2756</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2233</c:v>
+                    <c:v>0.2604</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0941</c:v>
+                    <c:v>0.3533</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1379,19 +1376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-14.0406</c:v>
+                  <c:v>17.353</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.8219</c:v>
+                  <c:v>31.5999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.885</c:v>
+                  <c:v>40.6926</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.0244</c:v>
+                  <c:v>45.6859</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.5051</c:v>
+                  <c:v>48.4321</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0578</c:v>
+                    <c:v>0.3082</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0663</c:v>
+                    <c:v>0.0892</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2967</c:v>
+                    <c:v>0.192</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.5364</c:v>
+                    <c:v>0.6262</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3538</c:v>
+                    <c:v>0.5172</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1464,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1163</c:v>
+                    <c:v>0.2714</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1244</c:v>
+                    <c:v>0.026</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2496</c:v>
+                    <c:v>0.2877</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4385</c:v>
+                    <c:v>0.6287</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4967</c:v>
+                    <c:v>0.6595</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1526,19 +1523,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3589</c:v>
+                  <c:v>0.451</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-16.6952</c:v>
+                  <c:v>7.1129</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.29</c:v>
+                  <c:v>24.5046</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.3413</c:v>
+                  <c:v>37.0812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.6712</c:v>
+                  <c:v>43.8981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1534</c:v>
+                    <c:v>0.1018</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.035</c:v>
+                    <c:v>0.1731</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2319</c:v>
+                    <c:v>0.5064</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0079</c:v>
+                    <c:v>0.8151</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8133</c:v>
+                    <c:v>0.7942</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1611,19 +1608,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0717</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0186</c:v>
+                    <c:v>0.1022</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0393</c:v>
+                    <c:v>1.6852</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.9691</c:v>
+                    <c:v>1.0027</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2046</c:v>
+                    <c:v>0.2587</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1676,16 +1673,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8349</c:v>
+                  <c:v>0.6751</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.6658</c:v>
+                  <c:v>13.0627</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.759</c:v>
+                  <c:v>25.7384</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.6785</c:v>
+                  <c:v>37.7166</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,19 +1731,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.1394</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0358</c:v>
+                    <c:v>0.4458</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2675</c:v>
+                    <c:v>0.2115</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6091</c:v>
+                    <c:v>0.1687</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6832</c:v>
+                    <c:v>0.2837</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1758,19 +1755,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.5441</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0191</c:v>
+                    <c:v>0.594</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1547</c:v>
+                    <c:v>1.1222</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.224</c:v>
+                    <c:v>0.1254</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4966</c:v>
+                    <c:v>0.3921</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1820,19 +1817,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.2059</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9563</c:v>
+                  <c:v>0.2445</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.7659</c:v>
+                  <c:v>7.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.4962</c:v>
+                  <c:v>28.2201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.7089</c:v>
+                  <c:v>39.0328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080122656"/>
-        <c:axId val="-2080116432"/>
+        <c:axId val="-2123740400"/>
+        <c:axId val="2051578576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2080122656"/>
+        <c:axId val="-2123740400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080116432"/>
+        <c:crossAx val="2051578576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2080116432"/>
+        <c:axId val="2051578576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080122656"/>
+        <c:crossAx val="-2123740400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,19 +2322,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>10.5025</c:v>
+                    <c:v>8.698</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.372</c:v>
+                    <c:v>0.3162</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.4601</c:v>
+                    <c:v>2.305</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0766</c:v>
+                    <c:v>0.0384</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0302</c:v>
+                    <c:v>0.2654</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,19 +2346,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0915</c:v>
+                    <c:v>0.083</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2004</c:v>
+                    <c:v>0.1703</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.4457</c:v>
+                    <c:v>8.7899</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.0913</c:v>
+                    <c:v>1.6423</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0993</c:v>
+                    <c:v>0.7895</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2411,19 +2408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-13.952</c:v>
+                  <c:v>17.353</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.1111</c:v>
+                  <c:v>49.696</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.77809999999999</c:v>
+                  <c:v>72.2136</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.8896</c:v>
+                  <c:v>85.4572</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92.4575</c:v>
+                  <c:v>92.2904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,19 +2469,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0578</c:v>
+                    <c:v>0.3082</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0663</c:v>
+                    <c:v>0.0892</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.6463</c:v>
+                    <c:v>5.8379</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.1541</c:v>
+                    <c:v>3.6945</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1282</c:v>
+                    <c:v>0.0349</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2496,19 +2493,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1163</c:v>
+                    <c:v>0.2714</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1244</c:v>
+                    <c:v>0.026</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>20.0491</c:v>
+                    <c:v>19.7777</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.0767</c:v>
+                    <c:v>0.1783</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.1133</c:v>
+                    <c:v>0.1311</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2558,19 +2555,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3589</c:v>
+                  <c:v>0.451</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-16.6952</c:v>
+                  <c:v>7.1129</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.5572</c:v>
+                  <c:v>46.6855</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69.1328</c:v>
+                  <c:v>73.4519</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.4428</c:v>
+                  <c:v>86.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,19 +2616,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1534</c:v>
+                    <c:v>0.1018</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.035</c:v>
+                    <c:v>0.1731</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.119</c:v>
+                    <c:v>4.8578</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.7739</c:v>
+                    <c:v>0.2363</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2384</c:v>
+                    <c:v>1.6682</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2643,19 +2640,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0717</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0186</c:v>
+                    <c:v>0.1022</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>12.0266</c:v>
+                    <c:v>12.4443</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.7136</c:v>
+                    <c:v>7.1685</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.2291</c:v>
+                    <c:v>5.7534</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2708,16 +2705,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8349</c:v>
+                  <c:v>0.6751</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.2844</c:v>
+                  <c:v>23.7676</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.4627</c:v>
+                  <c:v>56.2531</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.52800000000001</c:v>
+                  <c:v>76.2265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,19 +2763,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.1394</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0358</c:v>
+                    <c:v>0.4458</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.0133</c:v>
+                    <c:v>5.3012</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0736</c:v>
+                    <c:v>0.6316</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2385</c:v>
+                    <c:v>1.3387</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2790,19 +2787,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.5441</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0191</c:v>
+                    <c:v>0.594</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.7465</c:v>
+                    <c:v>12.876</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3985</c:v>
+                    <c:v>10.4278</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.843</c:v>
+                    <c:v>4.3785</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2852,19 +2849,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.2059</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9563</c:v>
+                  <c:v>0.2445</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.928000000000001</c:v>
+                  <c:v>19.3639</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.9358</c:v>
+                  <c:v>58.2975</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.4309</c:v>
+                  <c:v>77.7838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080041344"/>
-        <c:axId val="-2080035120"/>
+        <c:axId val="-2095311200"/>
+        <c:axId val="-2095304944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2080041344"/>
+        <c:axId val="-2095311200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,12 +2997,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080035120"/>
+        <c:crossAx val="-2095304944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2080035120"/>
+        <c:axId val="-2095304944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080041344"/>
+        <c:crossAx val="-2095311200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3357,19 +3354,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>9.7819</c:v>
+                    <c:v>9.9012</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4584</c:v>
+                    <c:v>0.4622</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.6685</c:v>
+                    <c:v>3.6915</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2402</c:v>
+                    <c:v>0.1385</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.098</c:v>
+                    <c:v>0.4416</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3384,16 +3381,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2468</c:v>
+                    <c:v>0.249</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>14.6745</c:v>
+                    <c:v>14.7622</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.51</c:v>
+                    <c:v>3.5625</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.1416</c:v>
+                    <c:v>1.556</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3446,16 +3443,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.2252</c:v>
+                  <c:v>26.4562</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.8768</c:v>
+                  <c:v>53.1686</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.8724</c:v>
+                  <c:v>73.2246</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85.3402</c:v>
+                  <c:v>85.0688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3510,13 +3507,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.9836</c:v>
+                    <c:v>7.5735</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6088</c:v>
+                    <c:v>6.2408</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4252</c:v>
+                    <c:v>0.1097</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3534,13 +3531,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>23.795</c:v>
+                    <c:v>26.5974</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.0089</c:v>
+                    <c:v>0.6162</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.2644</c:v>
+                    <c:v>0.1582</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3596,13 +3593,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.4447</c:v>
+                  <c:v>29.5339</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.4972</c:v>
+                  <c:v>57.7962</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73.2255</c:v>
+                  <c:v>76.2396</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3657,13 +3654,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.9489</c:v>
+                    <c:v>5.1351</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2315</c:v>
+                    <c:v>0.8162</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9242</c:v>
+                    <c:v>2.6814</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3681,13 +3678,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.8307</c:v>
+                    <c:v>12.346</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.0477</c:v>
+                    <c:v>8.4475</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.6803</c:v>
+                    <c:v>9.8499</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3743,13 +3740,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.7622</c:v>
+                  <c:v>12.2849</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.6003</c:v>
+                  <c:v>40.7987</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>62.4497</c:v>
+                  <c:v>61.8302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3804,13 +3801,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.9117</c:v>
+                    <c:v>5.5543</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2026</c:v>
+                    <c:v>0.8732</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6812</c:v>
+                    <c:v>2.0909</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3828,13 +3825,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.5511</c:v>
+                    <c:v>12.741</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3708</c:v>
+                    <c:v>14.6286</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.4666</c:v>
+                    <c:v>7.2544</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3890,13 +3887,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.491</c:v>
+                  <c:v>12.6653</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.6921</c:v>
+                  <c:v>42.0035</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>62.7354</c:v>
+                  <c:v>63.633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,11 +3908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079960048"/>
-        <c:axId val="-2079953824"/>
+        <c:axId val="-2094474784"/>
+        <c:axId val="-2094468528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2079960048"/>
+        <c:axId val="-2094474784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,12 +4029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079953824"/>
+        <c:crossAx val="-2094468528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2079953824"/>
+        <c:axId val="-2094468528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,7 +4164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079960048"/>
+        <c:crossAx val="-2094474784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6609,915 +6606,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>0</v>
-          </cell>
-          <cell r="F4">
-            <v>0.1643</v>
-          </cell>
-          <cell r="G4">
-            <v>2.8054999999999999</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>0</v>
-          </cell>
-          <cell r="F5">
-            <v>5.0853000000000002</v>
-          </cell>
-          <cell r="G5">
-            <v>1.5634999999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>0</v>
-          </cell>
-          <cell r="F6">
-            <v>3.8491</v>
-          </cell>
-          <cell r="G6">
-            <v>4.5976999999999997</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>0.99880000000000002</v>
-          </cell>
-          <cell r="F7">
-            <v>1.1251</v>
-          </cell>
-          <cell r="G7">
-            <v>1.5762</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>-1.0606</v>
-          </cell>
-          <cell r="F8">
-            <v>14.9473</v>
-          </cell>
-          <cell r="G8">
-            <v>0.85389999999999999</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>-1.5775999999999999</v>
-          </cell>
-          <cell r="F10">
-            <v>6.0461</v>
-          </cell>
-          <cell r="G10">
-            <v>7.6142000000000003</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>0</v>
-          </cell>
-          <cell r="F11">
-            <v>6.3746999999999998</v>
-          </cell>
-          <cell r="G11">
-            <v>4.8391999999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>0.47599999999999998</v>
-          </cell>
-          <cell r="F12">
-            <v>24.1937</v>
-          </cell>
-          <cell r="G12">
-            <v>4.7892999999999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>2.4679000000000002</v>
-          </cell>
-          <cell r="F13">
-            <v>7.1369999999999996</v>
-          </cell>
-          <cell r="G13">
-            <v>3.3473999999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>3.3096000000000001</v>
-          </cell>
-          <cell r="F14">
-            <v>4.7234999999999996</v>
-          </cell>
-          <cell r="G14">
-            <v>16.872199999999999</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-          <cell r="F16">
-            <v>3.7170000000000001</v>
-          </cell>
-          <cell r="G16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>-1.3613</v>
-          </cell>
-          <cell r="F17">
-            <v>8.2149999999999999</v>
-          </cell>
-          <cell r="G17">
-            <v>4.9702999999999999</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>0.4249</v>
-          </cell>
-          <cell r="F18">
-            <v>0.4249</v>
-          </cell>
-          <cell r="G18">
-            <v>12.2194</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>12.230700000000001</v>
-          </cell>
-          <cell r="F19">
-            <v>61.433300000000003</v>
-          </cell>
-          <cell r="G19">
-            <v>24.942699999999999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>-3.1762000000000001</v>
-          </cell>
-          <cell r="F20">
-            <v>42.6265</v>
-          </cell>
-          <cell r="G20">
-            <v>23.130800000000001</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>0</v>
-          </cell>
-          <cell r="F22">
-            <v>1.9496</v>
-          </cell>
-          <cell r="G22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>0</v>
-          </cell>
-          <cell r="F23">
-            <v>1.6688000000000001</v>
-          </cell>
-          <cell r="G23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>0.45829999999999999</v>
-          </cell>
-          <cell r="F24">
-            <v>3.8898999999999999</v>
-          </cell>
-          <cell r="G24">
-            <v>3.032</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>-1.6879</v>
-          </cell>
-          <cell r="F25">
-            <v>63.305999999999997</v>
-          </cell>
-          <cell r="G25">
-            <v>50.4649</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>-1.8727</v>
-          </cell>
-          <cell r="F26">
-            <v>11.662000000000001</v>
-          </cell>
-          <cell r="G26">
-            <v>23.3337</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>13.2614</v>
-          </cell>
-          <cell r="F29">
-            <v>1.8876999999999999</v>
-          </cell>
-          <cell r="G29">
-            <v>0.21709999999999999</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>9.6968999999999994</v>
-          </cell>
-          <cell r="F30">
-            <v>9.8062000000000005</v>
-          </cell>
-          <cell r="G30">
-            <v>3.1705000000000001</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>11.649900000000001</v>
-          </cell>
-          <cell r="F31">
-            <v>3.7254</v>
-          </cell>
-          <cell r="G31">
-            <v>6.0811999999999999</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>12.2293</v>
-          </cell>
-          <cell r="F32">
-            <v>0.94810000000000005</v>
-          </cell>
-          <cell r="G32">
-            <v>4.6520000000000001</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>12.5162</v>
-          </cell>
-          <cell r="F33">
-            <v>2.7187000000000001</v>
-          </cell>
-          <cell r="G33">
-            <v>1.0156000000000001</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>5.6441999999999997</v>
-          </cell>
-          <cell r="F35">
-            <v>5.6441999999999997</v>
-          </cell>
-          <cell r="G35">
-            <v>1.5902000000000001</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>12.847300000000001</v>
-          </cell>
-          <cell r="F36">
-            <v>12.8005</v>
-          </cell>
-          <cell r="G36">
-            <v>0.54349999999999998</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>10.454700000000001</v>
-          </cell>
-          <cell r="F37">
-            <v>15.8614</v>
-          </cell>
-          <cell r="G37">
-            <v>0.79569999999999996</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>16.051400000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>22.700700000000001</v>
-          </cell>
-          <cell r="G38">
-            <v>3.2416999999999998</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>15.5762</v>
-          </cell>
-          <cell r="F39">
-            <v>1.0969</v>
-          </cell>
-          <cell r="G39">
-            <v>18.361599999999999</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>0</v>
-          </cell>
-          <cell r="F41">
-            <v>0</v>
-          </cell>
-          <cell r="G41">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>0</v>
-          </cell>
-          <cell r="F42">
-            <v>0</v>
-          </cell>
-          <cell r="G42">
-            <v>6.8838999999999997</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>10.8827</v>
-          </cell>
-          <cell r="F43">
-            <v>4.3000999999999996</v>
-          </cell>
-          <cell r="G43">
-            <v>1.9446000000000001</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>15.3573</v>
-          </cell>
-          <cell r="F44">
-            <v>19.654399999999999</v>
-          </cell>
-          <cell r="G44">
-            <v>26.616199999999999</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>16.158799999999999</v>
-          </cell>
-          <cell r="F45">
-            <v>27.836600000000001</v>
-          </cell>
-          <cell r="G45">
-            <v>18.257000000000001</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0</v>
-          </cell>
-          <cell r="F47">
-            <v>0</v>
-          </cell>
-          <cell r="G47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>0</v>
-          </cell>
-          <cell r="F48">
-            <v>0</v>
-          </cell>
-          <cell r="G48">
-            <v>1.7171000000000001</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>1.5734999999999999</v>
-          </cell>
-          <cell r="F49">
-            <v>1.5734999999999999</v>
-          </cell>
-          <cell r="G49">
-            <v>3.6619999999999999</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>10.470499999999999</v>
-          </cell>
-          <cell r="F50">
-            <v>7.9917999999999996</v>
-          </cell>
-          <cell r="G50">
-            <v>44.195099999999996</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>9.7014999999999993</v>
-          </cell>
-          <cell r="F51">
-            <v>1.7801</v>
-          </cell>
-          <cell r="G51">
-            <v>32.2425</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>13.2614</v>
-          </cell>
-          <cell r="F54">
-            <v>1.8876999999999999</v>
-          </cell>
-          <cell r="G54">
-            <v>0.21709999999999999</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>11.326700000000001</v>
-          </cell>
-          <cell r="F55">
-            <v>11.436</v>
-          </cell>
-          <cell r="G55">
-            <v>1.923</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>40</v>
-          </cell>
-          <cell r="F56">
-            <v>9.5740999999999996</v>
-          </cell>
-          <cell r="G56">
-            <v>1.5264</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>60.003700000000002</v>
-          </cell>
-          <cell r="F57">
-            <v>0.55549999999999999</v>
-          </cell>
-          <cell r="G57">
-            <v>1.8740000000000001</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>77.846299999999999</v>
-          </cell>
-          <cell r="F58">
-            <v>4.8650000000000002</v>
-          </cell>
-          <cell r="G58">
-            <v>0.23069999999999999</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>5.6441999999999997</v>
-          </cell>
-          <cell r="F60">
-            <v>5.6441999999999997</v>
-          </cell>
-          <cell r="G60">
-            <v>1.5902000000000001</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>12.847300000000001</v>
-          </cell>
-          <cell r="F61">
-            <v>12.8005</v>
-          </cell>
-          <cell r="G61">
-            <v>0.54349999999999998</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>10.454700000000001</v>
-          </cell>
-          <cell r="F62">
-            <v>15.8614</v>
-          </cell>
-          <cell r="G62">
-            <v>0.79569999999999996</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>38.173999999999999</v>
-          </cell>
-          <cell r="F63">
-            <v>5.0109000000000004</v>
-          </cell>
-          <cell r="G63">
-            <v>6.3003</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>61.310600000000001</v>
-          </cell>
-          <cell r="F64">
-            <v>14.902100000000001</v>
-          </cell>
-          <cell r="G64">
-            <v>8.1167999999999996</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>0</v>
-          </cell>
-          <cell r="F66">
-            <v>0</v>
-          </cell>
-          <cell r="G66">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>0</v>
-          </cell>
-          <cell r="F67">
-            <v>0</v>
-          </cell>
-          <cell r="G67">
-            <v>6.8838999999999997</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>10.8827</v>
-          </cell>
-          <cell r="F68">
-            <v>4.3000999999999996</v>
-          </cell>
-          <cell r="G68">
-            <v>1.9446000000000001</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>26.523900000000001</v>
-          </cell>
-          <cell r="F69">
-            <v>23.739000000000001</v>
-          </cell>
-          <cell r="G69">
-            <v>16.110499999999998</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>24.443300000000001</v>
-          </cell>
-          <cell r="F70">
-            <v>33.001899999999999</v>
-          </cell>
-          <cell r="G70">
-            <v>16.8432</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>0</v>
-          </cell>
-          <cell r="F72">
-            <v>0</v>
-          </cell>
-          <cell r="G72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>0</v>
-          </cell>
-          <cell r="F73">
-            <v>0</v>
-          </cell>
-          <cell r="G73">
-            <v>1.7171000000000001</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>1.5734999999999999</v>
-          </cell>
-          <cell r="F74">
-            <v>1.5734999999999999</v>
-          </cell>
-          <cell r="G74">
-            <v>3.6619999999999999</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>8.6221999999999994</v>
-          </cell>
-          <cell r="F75">
-            <v>2.4939</v>
-          </cell>
-          <cell r="G75">
-            <v>49.9315</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>14.291700000000001</v>
-          </cell>
-          <cell r="F76">
-            <v>6.7023000000000001</v>
-          </cell>
-          <cell r="G76">
-            <v>24.596</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>0</v>
-          </cell>
-          <cell r="F79">
-            <v>0</v>
-          </cell>
-          <cell r="G79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>0</v>
-          </cell>
-          <cell r="F80">
-            <v>0</v>
-          </cell>
-          <cell r="G80">
-            <v>3.9342999999999999</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>27.0684</v>
-          </cell>
-          <cell r="F81">
-            <v>4.4432</v>
-          </cell>
-          <cell r="G81">
-            <v>5.7645999999999997</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>54.4985</v>
-          </cell>
-          <cell r="F82">
-            <v>1.7824</v>
-          </cell>
-          <cell r="G82">
-            <v>1.4715</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>74.558700000000002</v>
-          </cell>
-          <cell r="F83">
-            <v>5.8056999999999999</v>
-          </cell>
-          <cell r="G83">
-            <v>0.88129999999999997</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>0</v>
-          </cell>
-          <cell r="F85">
-            <v>0</v>
-          </cell>
-          <cell r="G85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>0</v>
-          </cell>
-          <cell r="F86">
-            <v>0</v>
-          </cell>
-          <cell r="G86">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>0</v>
-          </cell>
-          <cell r="F87">
-            <v>0</v>
-          </cell>
-          <cell r="G87">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>31.691500000000001</v>
-          </cell>
-          <cell r="F88">
-            <v>8.5687999999999995</v>
-          </cell>
-          <cell r="G88">
-            <v>9.1980000000000004</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>53.721400000000003</v>
-          </cell>
-          <cell r="F89">
-            <v>16.9374</v>
-          </cell>
-          <cell r="G89">
-            <v>1.2712000000000001</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0</v>
-          </cell>
-          <cell r="F91">
-            <v>0</v>
-          </cell>
-          <cell r="G91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>0</v>
-          </cell>
-          <cell r="F92">
-            <v>0</v>
-          </cell>
-          <cell r="G92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>0</v>
-          </cell>
-          <cell r="F93">
-            <v>0</v>
-          </cell>
-          <cell r="G93">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>8.9197000000000006</v>
-          </cell>
-          <cell r="F94">
-            <v>18.812200000000001</v>
-          </cell>
-          <cell r="G94">
-            <v>21.910599999999999</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>10.476100000000001</v>
-          </cell>
-          <cell r="F95">
-            <v>42.1678</v>
-          </cell>
-          <cell r="G95">
-            <v>22.694900000000001</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>0</v>
-          </cell>
-          <cell r="F97">
-            <v>0</v>
-          </cell>
-          <cell r="G97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>0</v>
-          </cell>
-          <cell r="F98">
-            <v>0</v>
-          </cell>
-          <cell r="G98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>0</v>
-          </cell>
-          <cell r="F99">
-            <v>0</v>
-          </cell>
-          <cell r="G99">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>0.31190000000000001</v>
-          </cell>
-          <cell r="F100">
-            <v>6.4145000000000003</v>
-          </cell>
-          <cell r="G100">
-            <v>8.2644000000000002</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>0.1547</v>
-          </cell>
-          <cell r="F101">
-            <v>7.9634999999999998</v>
-          </cell>
-          <cell r="G101">
-            <v>24.325700000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7786,7 +6874,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="Q83" sqref="Q83"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7853,10 +6941,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1.09E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G4">
-        <v>11.2164</v>
+        <v>8.1264000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7873,13 +6961,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>21.289100000000001</v>
+        <v>18.091200000000001</v>
       </c>
       <c r="F5">
-        <v>0.20030000000000001</v>
+        <v>0.17030000000000001</v>
       </c>
       <c r="G5">
-        <v>0.37209999999999999</v>
+        <v>0.31619999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7896,13 +6984,13 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <v>33.902000000000001</v>
+        <v>31.530200000000001</v>
       </c>
       <c r="F6">
-        <v>9.3802000000000003</v>
+        <v>8.7205999999999992</v>
       </c>
       <c r="G6">
-        <v>2.2229000000000001</v>
+        <v>2.0525000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7919,13 +7007,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>40.7117</v>
+        <v>39.9193</v>
       </c>
       <c r="F7">
-        <v>1.9919</v>
+        <v>1.8374999999999999</v>
       </c>
       <c r="G7">
-        <v>0.25169999999999998</v>
+        <v>0.12330000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7942,13 +7030,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>43.344999999999999</v>
+        <v>43.356000000000002</v>
       </c>
       <c r="F8">
-        <v>0.99</v>
+        <v>0.45040000000000002</v>
       </c>
       <c r="G8">
-        <v>0.87619999999999998</v>
+        <v>0.80549999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7965,13 +7053,13 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>-0.12609999999999999</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0.2233</v>
+        <v>0.26329999999999998</v>
       </c>
       <c r="G10">
-        <v>0.1164</v>
+        <v>0.37269999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7991,10 +7079,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>4.19E-2</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -8011,13 +7099,13 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>22.347200000000001</v>
+        <v>22.0488</v>
       </c>
       <c r="F12">
-        <v>20.129100000000001</v>
+        <v>19.795500000000001</v>
       </c>
       <c r="G12">
-        <v>5.6704999999999997</v>
+        <v>5.9688999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -8034,13 +7122,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>35.860799999999998</v>
+        <v>35.218899999999998</v>
       </c>
       <c r="F13">
-        <v>3.8769</v>
+        <v>2.5691000000000002</v>
       </c>
       <c r="G13">
-        <v>0.32400000000000001</v>
+        <v>1.1153999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8057,13 +7145,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>41.613799999999998</v>
+        <v>42.707000000000001</v>
       </c>
       <c r="F14">
-        <v>2.3435999999999999</v>
+        <v>1.9339999999999999</v>
       </c>
       <c r="G14">
-        <v>1.1987000000000001</v>
+        <v>0.23499999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -8080,10 +7168,10 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>-1.0800000000000001E-2</v>
       </c>
       <c r="F16">
-        <v>0.16900000000000001</v>
+        <v>0.18390000000000001</v>
       </c>
       <c r="G16">
         <v>0.15340000000000001</v>
@@ -8103,13 +7191,13 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.1013</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>0.1827</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>0.24199999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -8126,13 +7214,13 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>11.959199999999999</v>
+        <v>10.6767</v>
       </c>
       <c r="F18">
-        <v>12.0289</v>
+        <v>10.7309</v>
       </c>
       <c r="G18">
-        <v>5.1767000000000003</v>
+        <v>4.4358000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -8149,13 +7237,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>30.2959</v>
+        <v>29.652699999999999</v>
       </c>
       <c r="F19">
-        <v>5.9001000000000001</v>
+        <v>5.5403000000000002</v>
       </c>
       <c r="G19">
-        <v>0.49280000000000002</v>
+        <v>0.86629999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -8172,13 +7260,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>38.736400000000003</v>
+        <v>38.506900000000002</v>
       </c>
       <c r="F20">
-        <v>1.2189000000000001</v>
+        <v>1.8046</v>
       </c>
       <c r="G20">
-        <v>1.415</v>
+        <v>1.4903999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -8195,13 +7283,13 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.68910000000000005</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>0.65180000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -8218,13 +7306,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.40749999999999997</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.40749999999999997</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -8247,7 +7335,7 @@
         <v>11.7638</v>
       </c>
       <c r="G24">
-        <v>5.0774999999999997</v>
+        <v>5.0167999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -8264,13 +7352,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>30.4788</v>
+        <v>30.4207</v>
       </c>
       <c r="F25">
-        <v>7.7821999999999996</v>
+        <v>4.3144</v>
       </c>
       <c r="G25">
-        <v>0.81920000000000004</v>
+        <v>0.23150000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -8287,13 +7375,13 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>39.633200000000002</v>
+        <v>38.035800000000002</v>
       </c>
       <c r="F26">
-        <v>7.3163</v>
+        <v>1.5921000000000001</v>
       </c>
       <c r="G26">
-        <v>0.4113</v>
+        <v>2.1031</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -8318,13 +7406,13 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <v>-14.0406</v>
+        <v>17.353000000000002</v>
       </c>
       <c r="F29">
-        <v>0.62529999999999997</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="G29">
-        <v>9.1399999999999995E-2</v>
+        <v>0.57150000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -8341,7 +7429,7 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>18.821899999999999</v>
+        <v>31.599900000000002</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -8364,13 +7452,13 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>35.884999999999998</v>
+        <v>40.692599999999999</v>
       </c>
       <c r="F31">
-        <v>0.26400000000000001</v>
+        <v>0.27560000000000001</v>
       </c>
       <c r="G31">
-        <v>0.29559999999999997</v>
+        <v>0.31419999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -8387,13 +7475,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>44.0244</v>
+        <v>45.685899999999997</v>
       </c>
       <c r="F32">
-        <v>0.2233</v>
+        <v>0.26040000000000002</v>
       </c>
       <c r="G32">
-        <v>0.55669999999999997</v>
+        <v>0.96460000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -8410,13 +7498,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>48.505099999999999</v>
+        <v>48.432099999999998</v>
       </c>
       <c r="F33">
-        <v>9.4100000000000003E-2</v>
+        <v>0.3533</v>
       </c>
       <c r="G33">
-        <v>0.14050000000000001</v>
+        <v>0.25819999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -8433,13 +7521,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>0.3589</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="F35">
-        <v>0.1163</v>
+        <v>0.27139999999999997</v>
       </c>
       <c r="G35">
-        <v>5.7799999999999997E-2</v>
+        <v>0.30819999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -8456,13 +7544,13 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>-16.6952</v>
+        <v>7.1128999999999998</v>
       </c>
       <c r="F36">
-        <v>0.1244</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G36">
-        <v>6.6299999999999998E-2</v>
+        <v>8.9200000000000002E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -8479,13 +7567,13 @@
         <v>8</v>
       </c>
       <c r="E37">
-        <v>16.29</v>
+        <v>24.5046</v>
       </c>
       <c r="F37">
-        <v>0.24959999999999999</v>
+        <v>0.28770000000000001</v>
       </c>
       <c r="G37">
-        <v>0.29670000000000002</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -8502,13 +7590,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>33.341299999999997</v>
+        <v>37.081200000000003</v>
       </c>
       <c r="F38">
-        <v>0.4385</v>
+        <v>0.62870000000000004</v>
       </c>
       <c r="G38">
-        <v>0.53639999999999999</v>
+        <v>0.62619999999999998</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -8525,13 +7613,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>41.671199999999999</v>
+        <v>43.898099999999999</v>
       </c>
       <c r="F39">
-        <v>0.49669999999999997</v>
+        <v>0.65949999999999998</v>
       </c>
       <c r="G39">
-        <v>0.3538</v>
+        <v>0.51719999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -8551,10 +7639,10 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>7.17E-2</v>
       </c>
       <c r="G41">
-        <v>0.15340000000000001</v>
+        <v>0.1018</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -8571,13 +7659,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>5.8349000000000002</v>
+        <v>0.67510000000000003</v>
       </c>
       <c r="F42">
-        <v>1.8599999999999998E-2</v>
+        <v>0.1022</v>
       </c>
       <c r="G42">
-        <v>3.5000000000000003E-2</v>
+        <v>0.1731</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -8594,13 +7682,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>-1.6657999999999999</v>
+        <v>13.0627</v>
       </c>
       <c r="F43">
-        <v>3.9300000000000002E-2</v>
+        <v>1.6852</v>
       </c>
       <c r="G43">
-        <v>0.2319</v>
+        <v>0.50639999999999996</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -8617,13 +7705,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>23.759</v>
+        <v>25.738399999999999</v>
       </c>
       <c r="F44">
-        <v>0.96909999999999996</v>
+        <v>1.0026999999999999</v>
       </c>
       <c r="G44">
-        <v>1.0079</v>
+        <v>0.81510000000000005</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -8640,13 +7728,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>36.6785</v>
+        <v>37.7166</v>
       </c>
       <c r="F45">
-        <v>0.2046</v>
+        <v>0.25869999999999999</v>
       </c>
       <c r="G45">
-        <v>0.81330000000000002</v>
+        <v>0.79420000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -8663,13 +7751,13 @@
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>0.2059</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>0.54410000000000003</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>0.1394</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -8686,13 +7774,13 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>5.9562999999999997</v>
+        <v>0.2445</v>
       </c>
       <c r="F48">
-        <v>1.9099999999999999E-2</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="G48">
-        <v>3.5799999999999998E-2</v>
+        <v>0.44579999999999997</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -8709,13 +7797,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>-1.7659</v>
+        <v>7.67</v>
       </c>
       <c r="F49">
-        <v>0.1547</v>
+        <v>1.1222000000000001</v>
       </c>
       <c r="G49">
-        <v>0.26750000000000002</v>
+        <v>0.21149999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -8732,13 +7820,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>23.496200000000002</v>
+        <v>28.220099999999999</v>
       </c>
       <c r="F50">
-        <v>0.224</v>
+        <v>0.12540000000000001</v>
       </c>
       <c r="G50">
-        <v>0.60909999999999997</v>
+        <v>0.16869999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -8755,13 +7843,13 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>36.7089</v>
+        <v>39.032800000000002</v>
       </c>
       <c r="F51">
-        <v>0.49659999999999999</v>
+        <v>0.3921</v>
       </c>
       <c r="G51">
-        <v>0.68320000000000003</v>
+        <v>0.28370000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -8786,13 +7874,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>-13.952</v>
+        <v>17.353000000000002</v>
       </c>
       <c r="F54">
-        <v>9.1499999999999998E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="G54">
-        <v>10.5025</v>
+        <v>8.6980000000000004</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -8809,13 +7897,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>40.1111</v>
+        <v>49.695999999999998</v>
       </c>
       <c r="F55">
-        <v>0.20039999999999999</v>
+        <v>0.17030000000000001</v>
       </c>
       <c r="G55">
-        <v>0.372</v>
+        <v>0.31619999999999998</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -8832,13 +7920,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>69.778099999999995</v>
+        <v>72.2136</v>
       </c>
       <c r="F56">
-        <v>9.4457000000000004</v>
+        <v>8.7898999999999994</v>
       </c>
       <c r="G56">
-        <v>2.4601000000000002</v>
+        <v>2.3050000000000002</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -8855,13 +7943,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>84.889600000000002</v>
+        <v>85.4572</v>
       </c>
       <c r="F57">
-        <v>2.0912999999999999</v>
+        <v>1.6423000000000001</v>
       </c>
       <c r="G57">
-        <v>7.6600000000000001E-2</v>
+        <v>3.8399999999999997E-2</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -8878,13 +7966,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>92.457499999999996</v>
+        <v>92.290400000000005</v>
       </c>
       <c r="F58">
-        <v>1.0992999999999999</v>
+        <v>0.78949999999999998</v>
       </c>
       <c r="G58">
-        <v>3.0200000000000001E-2</v>
+        <v>0.26540000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -8901,13 +7989,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>0.3589</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="F60">
-        <v>0.1163</v>
+        <v>0.27139999999999997</v>
       </c>
       <c r="G60">
-        <v>5.7799999999999997E-2</v>
+        <v>0.30819999999999997</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8924,13 +8012,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>-16.6952</v>
+        <v>7.1128999999999998</v>
       </c>
       <c r="F61">
-        <v>0.1244</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G61">
-        <v>6.6299999999999998E-2</v>
+        <v>8.9200000000000002E-2</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8947,13 +8035,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>38.557200000000002</v>
+        <v>46.685499999999998</v>
       </c>
       <c r="F62">
-        <v>20.049099999999999</v>
+        <v>19.777699999999999</v>
       </c>
       <c r="G62">
-        <v>5.6463000000000001</v>
+        <v>5.8379000000000003</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8970,13 +8058,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>69.132800000000003</v>
+        <v>73.451899999999995</v>
       </c>
       <c r="F63">
-        <v>4.0766999999999998</v>
+        <v>0.17829999999999999</v>
       </c>
       <c r="G63">
-        <v>0.15409999999999999</v>
+        <v>3.6945000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8993,13 +8081,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>84.442800000000005</v>
+        <v>86.67</v>
       </c>
       <c r="F64">
-        <v>2.1133000000000002</v>
+        <v>0.13109999999999999</v>
       </c>
       <c r="G64">
-        <v>0.12820000000000001</v>
+        <v>3.49E-2</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9019,10 +8107,10 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>7.17E-2</v>
       </c>
       <c r="G66">
-        <v>0.15340000000000001</v>
+        <v>0.1018</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9039,13 +8127,13 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>5.8349000000000002</v>
+        <v>0.67510000000000003</v>
       </c>
       <c r="F67">
-        <v>1.8599999999999998E-2</v>
+        <v>0.1022</v>
       </c>
       <c r="G67">
-        <v>3.5000000000000003E-2</v>
+        <v>0.1731</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9062,13 +8150,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>10.2844</v>
+        <v>23.767600000000002</v>
       </c>
       <c r="F68">
-        <v>12.0266</v>
+        <v>12.4443</v>
       </c>
       <c r="G68">
-        <v>5.1189999999999998</v>
+        <v>4.8578000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9085,13 +8173,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>53.462699999999998</v>
+        <v>56.253100000000003</v>
       </c>
       <c r="F69">
-        <v>2.7136</v>
+        <v>7.1684999999999999</v>
       </c>
       <c r="G69">
-        <v>0.77390000000000003</v>
+        <v>0.23630000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9108,13 +8196,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>76.528000000000006</v>
+        <v>76.226500000000001</v>
       </c>
       <c r="F70">
-        <v>5.2290999999999999</v>
+        <v>5.7534000000000001</v>
       </c>
       <c r="G70">
-        <v>0.2384</v>
+        <v>1.6681999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9131,13 +8219,13 @@
         <v>2</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>0.2059</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>0.54410000000000003</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>0.1394</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -9154,13 +8242,13 @@
         <v>4</v>
       </c>
       <c r="E73">
-        <v>5.9562999999999997</v>
+        <v>0.2445</v>
       </c>
       <c r="F73">
-        <v>1.9099999999999999E-2</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="G73">
-        <v>3.5799999999999998E-2</v>
+        <v>0.44579999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -9177,13 +8265,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>9.9280000000000008</v>
+        <v>19.363900000000001</v>
       </c>
       <c r="F74">
-        <v>11.746499999999999</v>
+        <v>12.875999999999999</v>
       </c>
       <c r="G74">
-        <v>5.0133000000000001</v>
+        <v>5.3011999999999997</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9200,13 +8288,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>53.9358</v>
+        <v>58.297499999999999</v>
       </c>
       <c r="F75">
-        <v>0.39850000000000002</v>
+        <v>10.4278</v>
       </c>
       <c r="G75">
-        <v>7.3599999999999999E-2</v>
+        <v>0.63160000000000005</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +8311,13 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>76.430899999999994</v>
+        <v>77.783799999999999</v>
       </c>
       <c r="F76">
-        <v>2.843</v>
+        <v>4.3784999999999998</v>
       </c>
       <c r="G76">
-        <v>0.23849999999999999</v>
+        <v>1.3387</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9257,7 +8345,7 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>9.7819000000000003</v>
+        <v>9.9011999999999993</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -9274,13 +8362,13 @@
         <v>4</v>
       </c>
       <c r="E80">
-        <v>26.225200000000001</v>
+        <v>26.456199999999999</v>
       </c>
       <c r="F80">
-        <v>0.24679999999999999</v>
+        <v>0.249</v>
       </c>
       <c r="G80">
-        <v>0.45839999999999997</v>
+        <v>0.4622</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9297,13 +8385,13 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>52.876800000000003</v>
+        <v>53.168599999999998</v>
       </c>
       <c r="F81">
-        <v>14.6745</v>
+        <v>14.7622</v>
       </c>
       <c r="G81">
-        <v>3.6684999999999999</v>
+        <v>3.6915</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,13 +8408,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>72.872399999999999</v>
+        <v>73.224599999999995</v>
       </c>
       <c r="F82">
-        <v>3.51</v>
+        <v>3.5625</v>
       </c>
       <c r="G82">
-        <v>0.2402</v>
+        <v>0.13850000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,13 +8431,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>85.340199999999996</v>
+        <v>85.068799999999996</v>
       </c>
       <c r="F83">
-        <v>2.1415999999999999</v>
+        <v>1.556</v>
       </c>
       <c r="G83">
-        <v>9.8000000000000004E-2</v>
+        <v>0.44159999999999999</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9412,13 +8500,13 @@
         <v>8</v>
       </c>
       <c r="E87">
-        <v>26.444700000000001</v>
+        <v>29.533899999999999</v>
       </c>
       <c r="F87">
-        <v>23.795000000000002</v>
+        <v>26.5974</v>
       </c>
       <c r="G87">
-        <v>6.9836</v>
+        <v>7.5735000000000001</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,13 +8523,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>53.497199999999999</v>
+        <v>57.796199999999999</v>
       </c>
       <c r="F88">
-        <v>6.0088999999999997</v>
+        <v>0.61619999999999997</v>
       </c>
       <c r="G88">
-        <v>0.60880000000000001</v>
+        <v>6.2408000000000001</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,13 +8546,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>73.225499999999997</v>
+        <v>76.239599999999996</v>
       </c>
       <c r="F89">
-        <v>3.2644000000000002</v>
+        <v>0.15820000000000001</v>
       </c>
       <c r="G89">
-        <v>0.42520000000000002</v>
+        <v>0.10970000000000001</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -9527,13 +8615,13 @@
         <v>8</v>
       </c>
       <c r="E93">
-        <v>11.7622</v>
+        <v>12.2849</v>
       </c>
       <c r="F93">
-        <v>11.8307</v>
+        <v>12.346</v>
       </c>
       <c r="G93">
-        <v>4.9489000000000001</v>
+        <v>5.1351000000000004</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,13 +8638,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>39.600299999999997</v>
+        <v>40.798699999999997</v>
       </c>
       <c r="F94">
-        <v>4.0476999999999999</v>
+        <v>8.4474999999999998</v>
       </c>
       <c r="G94">
-        <v>0.23150000000000001</v>
+        <v>0.81620000000000004</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,13 +8661,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>62.4497</v>
+        <v>61.830199999999998</v>
       </c>
       <c r="F95">
-        <v>7.6802999999999999</v>
+        <v>9.8498999999999999</v>
       </c>
       <c r="G95">
-        <v>0.92420000000000002</v>
+        <v>2.6814</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -9642,13 +8730,13 @@
         <v>8</v>
       </c>
       <c r="E99">
-        <v>11.491</v>
+        <v>12.6653</v>
       </c>
       <c r="F99">
-        <v>11.5511</v>
+        <v>12.741</v>
       </c>
       <c r="G99">
-        <v>4.9116999999999997</v>
+        <v>5.5542999999999996</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,13 +8753,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>39.692100000000003</v>
+        <v>42.003500000000003</v>
       </c>
       <c r="F100">
-        <v>0.37080000000000002</v>
+        <v>14.6286</v>
       </c>
       <c r="G100">
-        <v>0.2026</v>
+        <v>0.87319999999999998</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,13 +8776,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>62.735399999999998</v>
+        <v>63.633000000000003</v>
       </c>
       <c r="F101">
-        <v>4.4665999999999997</v>
+        <v>7.2544000000000004</v>
       </c>
       <c r="G101">
-        <v>0.68120000000000003</v>
+        <v>2.0909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>